<commit_message>
some work on the dynamic stock modeling
</commit_message>
<xml_diff>
--- a/Data/regression_data/PpD/regression_PpD.xlsx
+++ b/Data/regression_data/PpD/regression_PpD.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B451"/>
+  <dimension ref="A1:B452"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2047,2001 +2047,2009 @@
     </row>
     <row r="202">
       <c r="A202" s="1" t="n">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="B202" t="n">
-        <v>5.308603967342242</v>
+        <v>5.31101693276688</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="1" t="n">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B203" t="n">
-        <v>5.30613196716526</v>
+        <v>5.308603967342242</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="1" t="n">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="B204" t="n">
-        <v>5.303599573312544</v>
+        <v>5.30613196716526</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="1" t="n">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="B205" t="n">
-        <v>5.301005399920881</v>
+        <v>5.303599573312544</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="1" t="n">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="B206" t="n">
-        <v>5.298348033877975</v>
+        <v>5.301005399920881</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="1" t="n">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="B207" t="n">
-        <v>5.295626034522412</v>
+        <v>5.298348033877975</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="1" t="n">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="B208" t="n">
-        <v>5.292837933353751</v>
+        <v>5.295626034522412</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="1" t="n">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="B209" t="n">
-        <v>5.289982233753726</v>
+        <v>5.292837933353751</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="1" t="n">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="B210" t="n">
-        <v>5.287057410719545</v>
+        <v>5.289982233753726</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="1" t="n">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="B211" t="n">
-        <v>5.284061910610365</v>
+        <v>5.287057410719545</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="1" t="n">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="B212" t="n">
-        <v>5.280994150908022</v>
+        <v>5.284061910610365</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="1" t="n">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="B213" t="n">
-        <v>5.277852519993197</v>
+        <v>5.280994150908022</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="1" t="n">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="B214" t="n">
-        <v>5.274635376938193</v>
+        <v>5.277852519993197</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="1" t="n">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="B215" t="n">
-        <v>5.271341051317592</v>
+        <v>5.274635376938193</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="1" t="n">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="B216" t="n">
-        <v>5.267967843038102</v>
+        <v>5.271341051317592</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="1" t="n">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="B217" t="n">
-        <v>5.264514022188933</v>
+        <v>5.267967843038102</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="1" t="n">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="B218" t="n">
-        <v>5.260977828914133</v>
+        <v>5.264514022188933</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="1" t="n">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="B219" t="n">
-        <v>5.257357473308353</v>
+        <v>5.260977828914133</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="1" t="n">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="B220" t="n">
-        <v>5.25365113533754</v>
+        <v>5.257357473308353</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="1" t="n">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="B221" t="n">
-        <v>5.249856964786161</v>
+        <v>5.25365113533754</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="1" t="n">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="B222" t="n">
-        <v>5.245973081232589</v>
+        <v>5.249856964786161</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="1" t="n">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="B223" t="n">
-        <v>5.241997574054323</v>
+        <v>5.245973081232589</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="1" t="n">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="B224" t="n">
-        <v>5.237928502464812</v>
+        <v>5.241997574054323</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="1" t="n">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="B225" t="n">
-        <v>5.233763895583682</v>
+        <v>5.237928502464812</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="1" t="n">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="B226" t="n">
-        <v>5.229501752542214</v>
+        <v>5.233763895583682</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="1" t="n">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="B227" t="n">
-        <v>5.22514004262601</v>
+        <v>5.229501752542214</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="1" t="n">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="B228" t="n">
-        <v>5.2206767054568</v>
+        <v>5.22514004262601</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="1" t="n">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="B229" t="n">
-        <v>5.216109651215435</v>
+        <v>5.2206767054568</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="1" t="n">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="B230" t="n">
-        <v>5.211436760908138</v>
+        <v>5.216109651215435</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="1" t="n">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="B231" t="n">
-        <v>5.206655886678141</v>
+        <v>5.211436760908138</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="1" t="n">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="B232" t="n">
-        <v>5.201764852164903</v>
+        <v>5.206655886678141</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="1" t="n">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="B233" t="n">
-        <v>5.196761452913138</v>
+        <v>5.201764852164903</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="1" t="n">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="B234" t="n">
-        <v>5.191643456833924</v>
+        <v>5.196761452913138</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="1" t="n">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="B235" t="n">
-        <v>5.186408604720234</v>
+        <v>5.191643456833924</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="1" t="n">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="B236" t="n">
-        <v>5.181054610819236</v>
+        <v>5.186408604720234</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" s="1" t="n">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="B237" t="n">
-        <v>5.175579163463767</v>
+        <v>5.181054610819236</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="1" t="n">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="B238" t="n">
-        <v>5.169979925765428</v>
+        <v>5.175579163463767</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" s="1" t="n">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="B239" t="n">
-        <v>5.164254536371759</v>
+        <v>5.169979925765428</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" s="1" t="n">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="B240" t="n">
-        <v>5.158400610289973</v>
+        <v>5.164254536371759</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" s="1" t="n">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="B241" t="n">
-        <v>5.152415739779783</v>
+        <v>5.158400610289973</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" s="1" t="n">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="B242" t="n">
-        <v>5.14629749531783</v>
+        <v>5.152415739779783</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" s="1" t="n">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="B243" t="n">
-        <v>5.140043426636253</v>
+        <v>5.14629749531783</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" s="1" t="n">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="B244" t="n">
-        <v>5.133651063837931</v>
+        <v>5.140043426636253</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" s="1" t="n">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="B245" t="n">
-        <v>5.127117918590937</v>
+        <v>5.133651063837931</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" s="1" t="n">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="B246" t="n">
-        <v>5.120441485404704</v>
+        <v>5.127117918590937</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" s="1" t="n">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="B247" t="n">
-        <v>5.113619242990418</v>
+        <v>5.120441485404704</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" s="1" t="n">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="B248" t="n">
-        <v>5.106648655708088</v>
+        <v>5.113619242990418</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="1" t="n">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="B249" t="n">
-        <v>5.099527175102715</v>
+        <v>5.106648655708088</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="1" t="n">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="B250" t="n">
-        <v>5.09225224153195</v>
+        <v>5.099527175102715</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" s="1" t="n">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="B251" t="n">
-        <v>5.084821285887529</v>
+        <v>5.09225224153195</v>
       </c>
     </row>
     <row r="252">
       <c r="A252" s="1" t="n">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="B252" t="n">
-        <v>5.077231731412745</v>
+        <v>5.084821285887529</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" s="1" t="n">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="B253" t="n">
-        <v>5.069480995618091</v>
+        <v>5.077231731412745</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" s="1" t="n">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="B254" t="n">
-        <v>5.061566492297147</v>
+        <v>5.069480995618091</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" s="1" t="n">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="B255" t="n">
-        <v>5.053485633644638</v>
+        <v>5.061566492297147</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" s="1" t="n">
-        <v>1855</v>
+        <v>1854</v>
       </c>
       <c r="B256" t="n">
-        <v>5.045235832478486</v>
+        <v>5.053485633644638</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" s="1" t="n">
-        <v>1856</v>
+        <v>1855</v>
       </c>
       <c r="B257" t="n">
-        <v>5.036814504567528</v>
+        <v>5.045235832478486</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" s="1" t="n">
-        <v>1857</v>
+        <v>1856</v>
       </c>
       <c r="B258" t="n">
-        <v>5.028219071066429</v>
+        <v>5.036814504567528</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" s="1" t="n">
-        <v>1858</v>
+        <v>1857</v>
       </c>
       <c r="B259" t="n">
-        <v>5.019446961059118</v>
+        <v>5.028219071066429</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" s="1" t="n">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="B260" t="n">
-        <v>5.010495614211912</v>
+        <v>5.019446961059118</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="1" t="n">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="B261" t="n">
-        <v>5.001362483537287</v>
+        <v>5.010495614211912</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" s="1" t="n">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="B262" t="n">
-        <v>4.992045038268998</v>
+        <v>5.001362483537287</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" s="1" t="n">
-        <v>1862</v>
+        <v>1861</v>
       </c>
       <c r="B263" t="n">
-        <v>4.982540766849047</v>
+        <v>4.992045038268998</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" s="1" t="n">
-        <v>1863</v>
+        <v>1862</v>
       </c>
       <c r="B264" t="n">
-        <v>4.972847180026712</v>
+        <v>4.982540766849047</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" s="1" t="n">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="B265" t="n">
-        <v>4.962961814069576</v>
+        <v>4.972847180026712</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" s="1" t="n">
-        <v>1865</v>
+        <v>1864</v>
       </c>
       <c r="B266" t="n">
-        <v>4.952882234086195</v>
+        <v>4.962961814069576</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" s="1" t="n">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="B267" t="n">
-        <v>4.942606037459713</v>
+        <v>4.952882234086195</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" s="1" t="n">
-        <v>1867</v>
+        <v>1866</v>
       </c>
       <c r="B268" t="n">
-        <v>4.932130857391431</v>
+        <v>4.942606037459713</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" s="1" t="n">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="B269" t="n">
-        <v>4.921454366552906</v>
+        <v>4.932130857391431</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" s="1" t="n">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="B270" t="n">
-        <v>4.910574280844868</v>
+        <v>4.921454366552906</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" s="1" t="n">
-        <v>1870</v>
+        <v>1869</v>
       </c>
       <c r="B271" t="n">
-        <v>4.899488363260748</v>
+        <v>4.910574280844868</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" s="1" t="n">
-        <v>1871</v>
+        <v>1870</v>
       </c>
       <c r="B272" t="n">
-        <v>4.888194427852292</v>
+        <v>4.899488363260748</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" s="1" t="n">
-        <v>1872</v>
+        <v>1871</v>
       </c>
       <c r="B273" t="n">
-        <v>4.876690343794187</v>
+        <v>4.888194427852292</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" s="1" t="n">
-        <v>1873</v>
+        <v>1872</v>
       </c>
       <c r="B274" t="n">
-        <v>4.8649740395443</v>
+        <v>4.876690343794187</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" s="1" t="n">
-        <v>1874</v>
+        <v>1873</v>
       </c>
       <c r="B275" t="n">
-        <v>4.853043507095521</v>
+        <v>4.8649740395443</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" s="1" t="n">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B276" t="n">
-        <v>4.840896806314833</v>
+        <v>4.853043507095521</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" s="1" t="n">
-        <v>1876</v>
+        <v>1875</v>
       </c>
       <c r="B277" t="n">
-        <v>4.828532069364639</v>
+        <v>4.840896806314833</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" s="1" t="n">
-        <v>1877</v>
+        <v>1876</v>
       </c>
       <c r="B278" t="n">
-        <v>4.815947505200907</v>
+        <v>4.828532069364639</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" s="1" t="n">
-        <v>1878</v>
+        <v>1877</v>
       </c>
       <c r="B279" t="n">
-        <v>4.803141404142149</v>
+        <v>4.815947505200907</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" s="1" t="n">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="B280" t="n">
-        <v>4.79011214250268</v>
+        <v>4.803141404142149</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" s="1" t="n">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="B281" t="n">
-        <v>4.776858187283105</v>
+        <v>4.79011214250268</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" s="1" t="n">
-        <v>1881</v>
+        <v>1880</v>
       </c>
       <c r="B282" t="n">
-        <v>4.763378100910353</v>
+        <v>4.776858187283105</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" s="1" t="n">
-        <v>1882</v>
+        <v>1881</v>
       </c>
       <c r="B283" t="n">
-        <v>4.749670546019067</v>
+        <v>4.763378100910353</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" s="1" t="n">
-        <v>1883</v>
+        <v>1882</v>
       </c>
       <c r="B284" t="n">
-        <v>4.735734290265553</v>
+        <v>4.749670546019067</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" s="1" t="n">
-        <v>1884</v>
+        <v>1883</v>
       </c>
       <c r="B285" t="n">
-        <v>4.721568211164931</v>
+        <v>4.735734290265553</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" s="1" t="n">
-        <v>1885</v>
+        <v>1884</v>
       </c>
       <c r="B286" t="n">
-        <v>4.707171300941569</v>
+        <v>4.721568211164931</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" s="1" t="n">
-        <v>1886</v>
+        <v>1885</v>
       </c>
       <c r="B287" t="n">
-        <v>4.692542671382292</v>
+        <v>4.707171300941569</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="1" t="n">
-        <v>1887</v>
+        <v>1886</v>
       </c>
       <c r="B288" t="n">
-        <v>4.677681558681334</v>
+        <v>4.692542671382292</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" s="1" t="n">
-        <v>1888</v>
+        <v>1887</v>
       </c>
       <c r="B289" t="n">
-        <v>4.662587328265424</v>
+        <v>4.677681558681334</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" s="1" t="n">
-        <v>1889</v>
+        <v>1888</v>
       </c>
       <c r="B290" t="n">
-        <v>4.647259479586889</v>
+        <v>4.662587328265424</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" s="1" t="n">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="B291" t="n">
-        <v>4.631697650872125</v>
+        <v>4.647259479586889</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" s="1" t="n">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="B292" t="n">
-        <v>4.615901623812312</v>
+        <v>4.631697650872125</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" s="1" t="n">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="B293" t="n">
-        <v>4.599871328182775</v>
+        <v>4.615901623812312</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" s="1" t="n">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="B294" t="n">
-        <v>4.58360684637696</v>
+        <v>4.599871328182775</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" s="1" t="n">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="B295" t="n">
-        <v>4.567108417840592</v>
+        <v>4.58360684637696</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" s="1" t="n">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="B296" t="n">
-        <v>4.550376443391213</v>
+        <v>4.567108417840592</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" s="1" t="n">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="B297" t="n">
-        <v>4.533411489407995</v>
+        <v>4.550376443391213</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" s="1" t="n">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="B298" t="n">
-        <v>4.516214291876429</v>
+        <v>4.533411489407995</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" s="1" t="n">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="B299" t="n">
-        <v>4.498785760272265</v>
+        <v>4.516214291876429</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" s="1" t="n">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="B300" t="n">
-        <v>4.481126981268933</v>
+        <v>4.498785760272265</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" s="1" t="n">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="B301" t="n">
-        <v>4.463239222252536</v>
+        <v>4.481126981268933</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" s="1" t="n">
-        <v>1901</v>
+        <v>1900</v>
       </c>
       <c r="B302" t="n">
-        <v>4.445123934628468</v>
+        <v>4.463239222252536</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="1" t="n">
-        <v>1902</v>
+        <v>1901</v>
       </c>
       <c r="B303" t="n">
-        <v>4.426782756903735</v>
+        <v>4.445123934628468</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="1" t="n">
-        <v>1903</v>
+        <v>1902</v>
       </c>
       <c r="B304" t="n">
-        <v>4.408217517529126</v>
+        <v>4.426782756903735</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" s="1" t="n">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="B305" t="n">
-        <v>4.389430237485549</v>
+        <v>4.408217517529126</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="1" t="n">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="B306" t="n">
-        <v>4.370423132599088</v>
+        <v>4.389430237485549</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" s="1" t="n">
-        <v>1906</v>
+        <v>1905</v>
       </c>
       <c r="B307" t="n">
-        <v>4.351198615569642</v>
+        <v>4.370423132599088</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="1" t="n">
-        <v>1907</v>
+        <v>1906</v>
       </c>
       <c r="B308" t="n">
-        <v>4.331759297698381</v>
+        <v>4.351198615569642</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="1" t="n">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="B309" t="n">
-        <v>4.312107990299769</v>
+        <v>4.331759297698381</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="1" t="n">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="B310" t="n">
-        <v>4.292247705784422</v>
+        <v>4.312107990299769</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="1" t="n">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="B311" t="n">
-        <v>4.272181658399738</v>
+        <v>4.292247705784422</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" s="1" t="n">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B312" t="n">
-        <v>4.251913264615932</v>
+        <v>4.272181658399738</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" s="1" t="n">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="B313" t="n">
-        <v>4.231446143145939</v>
+        <v>4.251913264615932</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="1" t="n">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="B314" t="n">
-        <v>4.210784114588544</v>
+        <v>4.231446143145939</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="1" t="n">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="B315" t="n">
-        <v>4.189931200685048</v>
+        <v>4.210784114588544</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="1" t="n">
-        <v>1915</v>
+        <v>1914</v>
       </c>
       <c r="B316" t="n">
-        <v>4.168891623180836</v>
+        <v>4.189931200685048</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" s="1" t="n">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="B317" t="n">
-        <v>4.147669802284367</v>
+        <v>4.168891623180836</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" s="1" t="n">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="B318" t="n">
-        <v>4.126270354717261</v>
+        <v>4.147669802284367</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" s="1" t="n">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="B319" t="n">
-        <v>4.104698091350477</v>
+        <v>4.126270354717261</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" s="1" t="n">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="B320" t="n">
-        <v>4.082958014422859</v>
+        <v>4.104698091350477</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="1" t="n">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="B321" t="n">
-        <v>4.061055314339756</v>
+        <v>4.082958014422859</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="1" t="n">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="B322" t="n">
-        <v>4.038995366050856</v>
+        <v>4.061055314339756</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" s="1" t="n">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="B323" t="n">
-        <v>4.01678372500785</v>
+        <v>4.038995366050856</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" s="1" t="n">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="B324" t="n">
-        <v>3.994426122704082</v>
+        <v>4.01678372500785</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="1" t="n">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="B325" t="n">
-        <v>3.971928461799905</v>
+        <v>3.994426122704082</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="1" t="n">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="B326" t="n">
-        <v>3.949296810839033</v>
+        <v>3.971928461799905</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="1" t="n">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="B327" t="n">
-        <v>3.926537398562781</v>
+        <v>3.949296810839033</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" s="1" t="n">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="B328" t="n">
-        <v>3.903656607830686</v>
+        <v>3.926537398562781</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="1" t="n">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="B329" t="n">
-        <v>3.880660969157599</v>
+        <v>3.903656607830686</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="1" t="n">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="B330" t="n">
-        <v>3.857557153878931</v>
+        <v>3.880660969157599</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" s="1" t="n">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="B331" t="n">
-        <v>3.834351966957268</v>
+        <v>3.857557153878931</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" s="1" t="n">
-        <v>1931</v>
+        <v>1930</v>
       </c>
       <c r="B332" t="n">
-        <v>3.811052339445144</v>
+        <v>3.834351966957268</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="1" t="n">
-        <v>1932</v>
+        <v>1931</v>
       </c>
       <c r="B333" t="n">
-        <v>3.787665320620204</v>
+        <v>3.811052339445144</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="1" t="n">
-        <v>1933</v>
+        <v>1932</v>
       </c>
       <c r="B334" t="n">
-        <v>3.764198069810444</v>
+        <v>3.787665320620204</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="1" t="n">
-        <v>1934</v>
+        <v>1933</v>
       </c>
       <c r="B335" t="n">
-        <v>3.740657847928597</v>
+        <v>3.764198069810444</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="1" t="n">
-        <v>1935</v>
+        <v>1934</v>
       </c>
       <c r="B336" t="n">
-        <v>3.717052008735998</v>
+        <v>3.740657847928597</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="1" t="n">
-        <v>1936</v>
+        <v>1935</v>
       </c>
       <c r="B337" t="n">
-        <v>3.693387989857533</v>
+        <v>3.717052008735998</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="1" t="n">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="B338" t="n">
-        <v>3.669673303570381</v>
+        <v>3.693387989857533</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="1" t="n">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="B339" t="n">
-        <v>3.645915527390293</v>
+        <v>3.669673303570381</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="1" t="n">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="B340" t="n">
-        <v>3.622122294480117</v>
+        <v>3.645915527390293</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" s="1" t="n">
-        <v>1940</v>
+        <v>1939</v>
       </c>
       <c r="B341" t="n">
-        <v>3.598301283906082</v>
+        <v>3.622122294480117</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" s="1" t="n">
-        <v>1941</v>
+        <v>1940</v>
       </c>
       <c r="B342" t="n">
-        <v>3.574460210768074</v>
+        <v>3.598301283906082</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="1" t="n">
-        <v>1942</v>
+        <v>1941</v>
       </c>
       <c r="B343" t="n">
-        <v>3.550606816230728</v>
+        <v>3.574460210768074</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" s="1" t="n">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="B344" t="n">
-        <v>3.526748857482626</v>
+        <v>3.550606816230728</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="1" t="n">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="B345" t="n">
-        <v>3.502894097651253</v>
+        <v>3.526748857482626</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="1" t="n">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="B346" t="n">
-        <v>3.479050295701518</v>
+        <v>3.502894097651253</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="1" t="n">
-        <v>1946</v>
+        <v>1945</v>
       </c>
       <c r="B347" t="n">
-        <v>3.455225196345799</v>
+        <v>3.479050295701518</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="1" t="n">
-        <v>1947</v>
+        <v>1946</v>
       </c>
       <c r="B348" t="n">
-        <v>3.431426519993346</v>
+        <v>3.455225196345799</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="1" t="n">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="B349" t="n">
-        <v>3.407661952766741</v>
+        <v>3.431426519993346</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="1" t="n">
-        <v>1949</v>
+        <v>1948</v>
       </c>
       <c r="B350" t="n">
-        <v>3.383939136612772</v>
+        <v>3.407661952766741</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="1" t="n">
-        <v>1950</v>
+        <v>1949</v>
       </c>
       <c r="B351" t="n">
-        <v>3.36026565953463</v>
+        <v>3.383939136612772</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="1" t="n">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="B352" t="n">
-        <v>3.336649045971784</v>
+        <v>3.36026565953463</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" s="1" t="n">
-        <v>1952</v>
+        <v>1951</v>
       </c>
       <c r="B353" t="n">
-        <v>3.313096747353187</v>
+        <v>3.336649045971784</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" s="1" t="n">
-        <v>1953</v>
+        <v>1952</v>
       </c>
       <c r="B354" t="n">
-        <v>3.289616132848653</v>
+        <v>3.313096747353187</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" s="1" t="n">
-        <v>1954</v>
+        <v>1953</v>
       </c>
       <c r="B355" t="n">
-        <v>3.26621448034234</v>
+        <v>3.289616132848653</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" s="1" t="n">
-        <v>1955</v>
+        <v>1954</v>
       </c>
       <c r="B356" t="n">
-        <v>3.242898967651244</v>
+        <v>3.26621448034234</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" s="1" t="n">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="B357" t="n">
-        <v>3.219676664010484</v>
+        <v>3.242898967651244</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" s="1" t="n">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="B358" t="n">
-        <v>3.19655452184597</v>
+        <v>3.219676664010484</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" s="1" t="n">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="B359" t="n">
-        <v>3.173539368853731</v>
+        <v>3.19655452184597</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" s="1" t="n">
-        <v>1959</v>
+        <v>1958</v>
       </c>
       <c r="B360" t="n">
-        <v>3.150637900403849</v>
+        <v>3.173539368853731</v>
       </c>
     </row>
     <row r="361">
       <c r="A361" s="1" t="n">
-        <v>1960</v>
+        <v>1959</v>
       </c>
       <c r="B361" t="n">
-        <v>3.127856672285478</v>
+        <v>3.150637900403849</v>
       </c>
     </row>
     <row r="362">
       <c r="A362" s="1" t="n">
-        <v>1961</v>
+        <v>1960</v>
       </c>
       <c r="B362" t="n">
-        <v>3.105202093808017</v>
+        <v>3.127856672285478</v>
       </c>
     </row>
     <row r="363">
       <c r="A363" s="1" t="n">
-        <v>1962</v>
+        <v>1961</v>
       </c>
       <c r="B363" t="n">
-        <v>3.082680421271898</v>
+        <v>3.105202093808017</v>
       </c>
     </row>
     <row r="364">
       <c r="A364" s="1" t="n">
-        <v>1963</v>
+        <v>1962</v>
       </c>
       <c r="B364" t="n">
-        <v>3.060297751820981</v>
+        <v>3.082680421271898</v>
       </c>
     </row>
     <row r="365">
       <c r="A365" s="1" t="n">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="B365" t="n">
-        <v>3.038060017686895</v>
+        <v>3.060297751820981</v>
       </c>
     </row>
     <row r="366">
       <c r="A366" s="1" t="n">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="B366" t="n">
-        <v>3.01597298083412</v>
+        <v>3.038060017686895</v>
       </c>
     </row>
     <row r="367">
       <c r="A367" s="1" t="n">
-        <v>1966</v>
+        <v>1965</v>
       </c>
       <c r="B367" t="n">
-        <v>2.994042228012976</v>
+        <v>3.01597298083412</v>
       </c>
     </row>
     <row r="368">
       <c r="A368" s="1" t="n">
-        <v>1967</v>
+        <v>1966</v>
       </c>
       <c r="B368" t="n">
-        <v>2.972273166226091</v>
+        <v>2.994042228012976</v>
       </c>
     </row>
     <row r="369">
       <c r="A369" s="1" t="n">
-        <v>1968</v>
+        <v>1967</v>
       </c>
       <c r="B369" t="n">
-        <v>2.950671018612337</v>
+        <v>2.972273166226091</v>
       </c>
     </row>
     <row r="370">
       <c r="A370" s="1" t="n">
-        <v>1969</v>
+        <v>1968</v>
       </c>
       <c r="B370" t="n">
-        <v>2.92924082075068</v>
+        <v>2.950671018612337</v>
       </c>
     </row>
     <row r="371">
       <c r="A371" s="1" t="n">
-        <v>1970</v>
+        <v>1969</v>
       </c>
       <c r="B371" t="n">
-        <v>2.907987417384801</v>
+        <v>2.92924082075068</v>
       </c>
     </row>
     <row r="372">
       <c r="A372" s="1" t="n">
-        <v>1971</v>
+        <v>1970</v>
       </c>
       <c r="B372" t="n">
-        <v>2.886915459567919</v>
+        <v>2.907987417384801</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" s="1" t="n">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="B373" t="n">
-        <v>2.866029402225734</v>
+        <v>2.886915459567919</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" s="1" t="n">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="B374" t="n">
-        <v>2.845333502134044</v>
+        <v>2.866029402225734</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" s="1" t="n">
-        <v>1974</v>
+        <v>1973</v>
       </c>
       <c r="B375" t="n">
-        <v>2.824831816306233</v>
+        <v>2.845333502134044</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" s="1" t="n">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="B376" t="n">
-        <v>2.804528200784545</v>
+        <v>2.824831816306233</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" s="1" t="n">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="B377" t="n">
-        <v>2.784426309827849</v>
+        <v>2.804528200784545</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" s="1" t="n">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="B378" t="n">
-        <v>2.764529595487465</v>
+        <v>2.784426309827849</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" s="1" t="n">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="B379" t="n">
-        <v>2.744841307561546</v>
+        <v>2.764529595487465</v>
       </c>
     </row>
     <row r="380">
       <c r="A380" s="1" t="n">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="B380" t="n">
-        <v>2.725364493917528</v>
+        <v>2.744841307561546</v>
       </c>
     </row>
     <row r="381">
       <c r="A381" s="1" t="n">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="B381" t="n">
-        <v>2.706102001171264</v>
+        <v>2.725364493917528</v>
       </c>
     </row>
     <row r="382">
       <c r="A382" s="1" t="n">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="B382" t="n">
-        <v>2.687056475710611</v>
+        <v>2.706102001171264</v>
       </c>
     </row>
     <row r="383">
       <c r="A383" s="1" t="n">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="B383" t="n">
-        <v>2.668230365050541</v>
+        <v>2.687056475710611</v>
       </c>
     </row>
     <row r="384">
       <c r="A384" s="1" t="n">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="B384" t="n">
-        <v>2.649625919506134</v>
+        <v>2.668230365050541</v>
       </c>
     </row>
     <row r="385">
       <c r="A385" s="1" t="n">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="B385" t="n">
-        <v>2.631245194169299</v>
+        <v>2.649625919506134</v>
       </c>
     </row>
     <row r="386">
       <c r="A386" s="1" t="n">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="B386" t="n">
-        <v>2.613090051174539</v>
+        <v>2.631245194169299</v>
       </c>
     </row>
     <row r="387">
       <c r="A387" s="1" t="n">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="B387" t="n">
-        <v>2.595162162238684</v>
+        <v>2.613090051174539</v>
       </c>
     </row>
     <row r="388">
       <c r="A388" s="1" t="n">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="B388" t="n">
-        <v>2.577463011459201</v>
+        <v>2.595162162238684</v>
       </c>
     </row>
     <row r="389">
       <c r="A389" s="1" t="n">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="B389" t="n">
-        <v>2.559993898355414</v>
+        <v>2.577463011459201</v>
       </c>
     </row>
     <row r="390">
       <c r="A390" s="1" t="n">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="B390" t="n">
-        <v>2.542755941136824</v>
+        <v>2.559993898355414</v>
       </c>
     </row>
     <row r="391">
       <c r="A391" s="1" t="n">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B391" t="n">
-        <v>2.525750080182612</v>
+        <v>2.542755941136824</v>
       </c>
     </row>
     <row r="392">
       <c r="A392" s="1" t="n">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="B392" t="n">
-        <v>2.508977081716364</v>
+        <v>2.525750080182612</v>
       </c>
     </row>
     <row r="393">
       <c r="A393" s="1" t="n">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="B393" t="n">
-        <v>2.492437541660117</v>
+        <v>2.508977081716364</v>
       </c>
     </row>
     <row r="394">
       <c r="A394" s="1" t="n">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B394" t="n">
-        <v>2.476131889651908</v>
+        <v>2.492437541660117</v>
       </c>
     </row>
     <row r="395">
       <c r="A395" s="1" t="n">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B395" t="n">
-        <v>2.460060393211182</v>
+        <v>2.476131889651908</v>
       </c>
     </row>
     <row r="396">
       <c r="A396" s="1" t="n">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B396" t="n">
-        <v>2.444223162036621</v>
+        <v>2.460060393211182</v>
       </c>
     </row>
     <row r="397">
       <c r="A397" s="1" t="n">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="B397" t="n">
-        <v>2.428620152421225</v>
+        <v>2.444223162036621</v>
       </c>
     </row>
     <row r="398">
       <c r="A398" s="1" t="n">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="B398" t="n">
-        <v>2.413251171769781</v>
+        <v>2.428620152421225</v>
       </c>
     </row>
     <row r="399">
       <c r="A399" s="1" t="n">
-        <v>1998</v>
+        <v>1997</v>
       </c>
       <c r="B399" t="n">
-        <v>2.398115883204246</v>
+        <v>2.413251171769781</v>
       </c>
     </row>
     <row r="400">
       <c r="A400" s="1" t="n">
-        <v>1999</v>
+        <v>1998</v>
       </c>
       <c r="B400" t="n">
-        <v>2.383213810242894</v>
+        <v>2.398115883204246</v>
       </c>
     </row>
     <row r="401">
       <c r="A401" s="1" t="n">
-        <v>2000</v>
+        <v>1999</v>
       </c>
       <c r="B401" t="n">
-        <v>2.36854434153961</v>
+        <v>2.383213810242894</v>
       </c>
     </row>
     <row r="402">
       <c r="A402" s="1" t="n">
-        <v>2001</v>
+        <v>2000</v>
       </c>
       <c r="B402" t="n">
-        <v>2.354106735670065</v>
+        <v>2.36854434153961</v>
       </c>
     </row>
     <row r="403">
       <c r="A403" s="1" t="n">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="B403" t="n">
-        <v>2.339900125952069</v>
+        <v>2.354106735670065</v>
       </c>
     </row>
     <row r="404">
       <c r="A404" s="1" t="n">
-        <v>2003</v>
+        <v>2002</v>
       </c>
       <c r="B404" t="n">
-        <v>2.325923525287887</v>
+        <v>2.339900125952069</v>
       </c>
     </row>
     <row r="405">
       <c r="A405" s="1" t="n">
-        <v>2004</v>
+        <v>2003</v>
       </c>
       <c r="B405" t="n">
-        <v>2.312175831016815</v>
+        <v>2.325923525287887</v>
       </c>
     </row>
     <row r="406">
       <c r="A406" s="1" t="n">
-        <v>2005</v>
+        <v>2004</v>
       </c>
       <c r="B406" t="n">
-        <v>2.298655829766871</v>
+        <v>2.312175831016815</v>
       </c>
     </row>
     <row r="407">
       <c r="A407" s="1" t="n">
-        <v>2006</v>
+        <v>2005</v>
       </c>
       <c r="B407" t="n">
-        <v>2.285362202295028</v>
+        <v>2.298655829766871</v>
       </c>
     </row>
     <row r="408">
       <c r="A408" s="1" t="n">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B408" t="n">
-        <v>2.272293528305926</v>
+        <v>2.285362202295028</v>
       </c>
     </row>
     <row r="409">
       <c r="A409" s="1" t="n">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="B409" t="n">
-        <v>2.259448291239654</v>
+        <v>2.272293528305926</v>
       </c>
     </row>
     <row r="410">
       <c r="A410" s="1" t="n">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B410" t="n">
-        <v>2.246824883019661</v>
+        <v>2.259448291239654</v>
       </c>
     </row>
     <row r="411">
       <c r="A411" s="1" t="n">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="B411" t="n">
-        <v>2.234421608752533</v>
+        <v>2.246824883019661</v>
       </c>
     </row>
     <row r="412">
       <c r="A412" s="1" t="n">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B412" t="n">
-        <v>2.222236691371843</v>
+        <v>2.234421608752533</v>
       </c>
     </row>
     <row r="413">
       <c r="A413" s="1" t="n">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B413" t="n">
-        <v>2.210268276218929</v>
+        <v>2.222236691371843</v>
       </c>
     </row>
     <row r="414">
       <c r="A414" s="1" t="n">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="B414" t="n">
-        <v>2.198514435553944</v>
+        <v>2.210268276218929</v>
       </c>
     </row>
     <row r="415">
       <c r="A415" s="1" t="n">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B415" t="n">
-        <v>2.186973172991109</v>
+        <v>2.198514435553944</v>
       </c>
     </row>
     <row r="416">
       <c r="A416" s="1" t="n">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="B416" t="n">
-        <v>2.175642427852615</v>
+        <v>2.186973172991109</v>
       </c>
     </row>
     <row r="417">
       <c r="A417" s="1" t="n">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B417" t="n">
-        <v>2.164520079436155</v>
+        <v>2.175642427852615</v>
       </c>
     </row>
     <row r="418">
       <c r="A418" s="1" t="n">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B418" t="n">
-        <v>2.153603951191561</v>
+        <v>2.164520079436155</v>
       </c>
     </row>
     <row r="419">
       <c r="A419" s="1" t="n">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="B419" t="n">
-        <v>2.142891814802526</v>
+        <v>2.153603951191561</v>
       </c>
     </row>
     <row r="420">
       <c r="A420" s="1" t="n">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B420" t="n">
-        <v>2.132381394169848</v>
+        <v>2.142891814802526</v>
       </c>
     </row>
     <row r="421">
       <c r="A421" s="1" t="n">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="B421" t="n">
-        <v>2.122070369293131</v>
+        <v>2.132381394169848</v>
       </c>
     </row>
     <row r="422">
       <c r="A422" s="1" t="n">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="B422" t="n">
-        <v>2.111956380048251</v>
+        <v>2.122070369293131</v>
       </c>
     </row>
     <row r="423">
       <c r="A423" s="1" t="n">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="B423" t="n">
-        <v>2.1020370298584</v>
+        <v>2.111956380048251</v>
       </c>
     </row>
     <row r="424">
       <c r="A424" s="1" t="n">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B424" t="n">
-        <v>2.092309889256838</v>
+        <v>2.1020370298584</v>
       </c>
     </row>
     <row r="425">
       <c r="A425" s="1" t="n">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B425" t="n">
-        <v>2.082772499339941</v>
+        <v>2.092309889256838</v>
       </c>
     </row>
     <row r="426">
       <c r="A426" s="1" t="n">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="B426" t="n">
-        <v>2.073422375109441</v>
+        <v>2.082772499339941</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="1" t="n">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="B427" t="n">
-        <v>2.064257008703124</v>
+        <v>2.073422375109441</v>
       </c>
     </row>
     <row r="428">
       <c r="A428" s="1" t="n">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="B428" t="n">
-        <v>2.055273872513574</v>
+        <v>2.064257008703124</v>
       </c>
     </row>
     <row r="429">
       <c r="A429" s="1" t="n">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="B429" t="n">
-        <v>2.046470422194838</v>
+        <v>2.055273872513574</v>
       </c>
     </row>
     <row r="430">
       <c r="A430" s="1" t="n">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="B430" t="n">
-        <v>2.037844099557196</v>
+        <v>2.046470422194838</v>
       </c>
     </row>
     <row r="431">
       <c r="A431" s="1" t="n">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="B431" t="n">
-        <v>2.02939233535047</v>
+        <v>2.037844099557196</v>
       </c>
     </row>
     <row r="432">
       <c r="A432" s="1" t="n">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="B432" t="n">
-        <v>2.021112551936541</v>
+        <v>2.02939233535047</v>
       </c>
     </row>
     <row r="433">
       <c r="A433" s="1" t="n">
-        <v>2032</v>
+        <v>2031</v>
       </c>
       <c r="B433" t="n">
-        <v>2.013002165852012</v>
+        <v>2.021112551936541</v>
       </c>
     </row>
     <row r="434">
       <c r="A434" s="1" t="n">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="B434" t="n">
-        <v>2.005058590262103</v>
+        <v>2.013002165852012</v>
       </c>
     </row>
     <row r="435">
       <c r="A435" s="1" t="n">
-        <v>2034</v>
+        <v>2033</v>
       </c>
       <c r="B435" t="n">
-        <v>1.997279237307128</v>
+        <v>2.005058590262103</v>
       </c>
     </row>
     <row r="436">
       <c r="A436" s="1" t="n">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="B436" t="n">
-        <v>1.989661520343006</v>
+        <v>1.997279237307128</v>
       </c>
     </row>
     <row r="437">
       <c r="A437" s="1" t="n">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="B437" t="n">
-        <v>1.982202856077495</v>
+        <v>1.989661520343006</v>
       </c>
     </row>
     <row r="438">
       <c r="A438" s="1" t="n">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="B438" t="n">
-        <v>1.974900666603898</v>
+        <v>1.982202856077495</v>
       </c>
     </row>
     <row r="439">
       <c r="A439" s="1" t="n">
-        <v>2038</v>
+        <v>2037</v>
       </c>
       <c r="B439" t="n">
-        <v>1.967752381334202</v>
+        <v>1.974900666603898</v>
       </c>
     </row>
     <row r="440">
       <c r="A440" s="1" t="n">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="B440" t="n">
-        <v>1.96075543883366</v>
+        <v>1.967752381334202</v>
       </c>
     </row>
     <row r="441">
       <c r="A441" s="1" t="n">
-        <v>2040</v>
+        <v>2039</v>
       </c>
       <c r="B441" t="n">
-        <v>1.953907288558957</v>
+        <v>1.96075543883366</v>
       </c>
     </row>
     <row r="442">
       <c r="A442" s="1" t="n">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="B442" t="n">
-        <v>1.947205392502198</v>
+        <v>1.953907288558957</v>
       </c>
     </row>
     <row r="443">
       <c r="A443" s="1" t="n">
-        <v>2042</v>
+        <v>2041</v>
       </c>
       <c r="B443" t="n">
-        <v>1.940647226742998</v>
+        <v>1.947205392502198</v>
       </c>
     </row>
     <row r="444">
       <c r="A444" s="1" t="n">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="B444" t="n">
-        <v>1.934230282911051</v>
+        <v>1.940647226742998</v>
       </c>
     </row>
     <row r="445">
       <c r="A445" s="1" t="n">
-        <v>2044</v>
+        <v>2043</v>
       </c>
       <c r="B445" t="n">
-        <v>1.927952069561586</v>
+        <v>1.934230282911051</v>
       </c>
     </row>
     <row r="446">
       <c r="A446" s="1" t="n">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="B446" t="n">
-        <v>1.921810113466171</v>
+        <v>1.927952069561586</v>
       </c>
     </row>
     <row r="447">
       <c r="A447" s="1" t="n">
-        <v>2046</v>
+        <v>2045</v>
       </c>
       <c r="B447" t="n">
-        <v>1.915801960821359</v>
+        <v>1.921810113466171</v>
       </c>
     </row>
     <row r="448">
       <c r="A448" s="1" t="n">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="B448" t="n">
-        <v>1.909925178377672</v>
+        <v>1.915801960821359</v>
       </c>
     </row>
     <row r="449">
       <c r="A449" s="1" t="n">
-        <v>2048</v>
+        <v>2047</v>
       </c>
       <c r="B449" t="n">
-        <v>1.904177354491483</v>
+        <v>1.909925178377672</v>
       </c>
     </row>
     <row r="450">
       <c r="A450" s="1" t="n">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="B450" t="n">
-        <v>1.898556100102293</v>
+        <v>1.904177354491483</v>
       </c>
     </row>
     <row r="451">
       <c r="A451" s="1" t="n">
+        <v>2049</v>
+      </c>
+      <c r="B451" t="n">
+        <v>1.898556100102293</v>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" s="1" t="n">
         <v>2050</v>
       </c>
-      <c r="B451" t="n">
+      <c r="B452" t="n">
         <v>1.893059049637972</v>
       </c>
     </row>

</xml_diff>